<commit_message>
modified:   Hairstyle_counts.xlsx 	modified:   Scripts/Return as JSON Objects/Betaface_23:type [21 - 40] 	modified:   Scripts/Return as JSON Objects/Betaface_23:type [41 - 61]
</commit_message>
<xml_diff>
--- a/Hairstyle_counts.xlsx
+++ b/Hairstyle_counts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p.xing/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p.xing/Hairstyle60k/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7511C14F-397E-D64B-B72B-F945A30DE718}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0183D85C-7E42-CD4D-A8F0-20827DC0F9FC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2960" yWindow="460" windowWidth="18720" windowHeight="17040" xr2:uid="{CA16EC3B-66EC-3C44-819A-9CA41E110A47}"/>
   </bookViews>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B46549-24DB-F147-A6C4-3602763BDF26}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add a sample image
</commit_message>
<xml_diff>
--- a/Hairstyle_counts.xlsx
+++ b/Hairstyle_counts.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p.xing/Hairstyle60k/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarkxing/Downloads/Hairstyle60k/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C49EBF-B372-BC4C-81EE-6BC5A895C6AB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC01F238-2228-164F-9CE2-7031E93E4D08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="460" windowWidth="18720" windowHeight="17040" xr2:uid="{CA16EC3B-66EC-3C44-819A-9CA41E110A47}"/>
+    <workbookView xWindow="5020" yWindow="460" windowWidth="18720" windowHeight="15540" xr2:uid="{CA16EC3B-66EC-3C44-819A-9CA41E110A47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Aaron_Kwok</t>
   </si>
@@ -214,186 +214,6 @@
   </si>
   <si>
     <t>Skipped</t>
-  </si>
-  <si>
-    <t>Wave_Hair.json</t>
-  </si>
-  <si>
-    <t>Aaron_Kwok.json</t>
-  </si>
-  <si>
-    <t>Afro.json</t>
-  </si>
-  <si>
-    <t>Bald.json</t>
-  </si>
-  <si>
-    <t>BeehiveBob.json</t>
-  </si>
-  <si>
-    <t>Bouffant.json</t>
-  </si>
-  <si>
-    <t>Bowl_Cut.json</t>
-  </si>
-  <si>
-    <t>Bun.json</t>
-  </si>
-  <si>
-    <t>Caesar.json</t>
-  </si>
-  <si>
-    <t>Chonmage.json</t>
-  </si>
-  <si>
-    <t>Comb_Over.json</t>
-  </si>
-  <si>
-    <t>Cornrows.json</t>
-  </si>
-  <si>
-    <t>Crew_Cut.json</t>
-  </si>
-  <si>
-    <t>Crop.json</t>
-  </si>
-  <si>
-    <t>Croydon_Facelift.json</t>
-  </si>
-  <si>
-    <t>Curly_Hair.json</t>
-  </si>
-  <si>
-    <t>Curly.json</t>
-  </si>
-  <si>
-    <t>Curtained_Hair.json</t>
-  </si>
-  <si>
-    <t>Cute_Ponytails.json</t>
-  </si>
-  <si>
-    <t>Devilock.json</t>
-  </si>
-  <si>
-    <t>Dreadlocks.json</t>
-  </si>
-  <si>
-    <t>Ducktail.json</t>
-  </si>
-  <si>
-    <t>Emo_hair.json</t>
-  </si>
-  <si>
-    <t>Fauxhawk.json</t>
-  </si>
-  <si>
-    <t>Flattop.json</t>
-  </si>
-  <si>
-    <t>French_Braid.json</t>
-  </si>
-  <si>
-    <t>French_Twist.json</t>
-  </si>
-  <si>
-    <t>Hi-top_Fade.json</t>
-  </si>
-  <si>
-    <t>Hime_Cut.json</t>
-  </si>
-  <si>
-    <t>Horseshoe_Flattop.json</t>
-  </si>
-  <si>
-    <t>Induction_Cut.json</t>
-  </si>
-  <si>
-    <t>Jimmy_Lin_Hairstyle.json</t>
-  </si>
-  <si>
-    <t>Layered_Hair.json</t>
-  </si>
-  <si>
-    <t>Liberty_Spikes_Hair.json</t>
-  </si>
-  <si>
-    <t>Long_Hair.json</t>
-  </si>
-  <si>
-    <t>Medium-Length_Hair.json</t>
-  </si>
-  <si>
-    <t>Men_Pompadour.json</t>
-  </si>
-  <si>
-    <t>Men_With_Square_Angles.json</t>
-  </si>
-  <si>
-    <t>Mohawk.json</t>
-  </si>
-  <si>
-    <t>Mop-Top_Hair.json</t>
-  </si>
-  <si>
-    <t>Mullet.json</t>
-  </si>
-  <si>
-    <t>Odango_Hair.json</t>
-  </si>
-  <si>
-    <t>Pageboy.json</t>
-  </si>
-  <si>
-    <t>Perm.json</t>
-  </si>
-  <si>
-    <t>Pixie_Cut.json</t>
-  </si>
-  <si>
-    <t>Ponytail.json</t>
-  </si>
-  <si>
-    <t>Quiff.json</t>
-  </si>
-  <si>
-    <t>Rattail.json</t>
-  </si>
-  <si>
-    <t>Razor_Cut.json</t>
-  </si>
-  <si>
-    <t>Ringlet.json</t>
-  </si>
-  <si>
-    <t>Shag.json</t>
-  </si>
-  <si>
-    <t>Shoulder-Length_Hair.json</t>
-  </si>
-  <si>
-    <t>Side_Part.json</t>
-  </si>
-  <si>
-    <t>Slicked-back.json</t>
-  </si>
-  <si>
-    <t>Spiky_Hair.json</t>
-  </si>
-  <si>
-    <t>Tapered_Sides.json</t>
-  </si>
-  <si>
-    <t>The_Rachel.json</t>
-  </si>
-  <si>
-    <t>Tonsure_Hair.json</t>
-  </si>
-  <si>
-    <t>Updo.json</t>
-  </si>
-  <si>
-    <t>Waist-Length_Hair.json</t>
   </si>
 </sst>
 </file>
@@ -409,12 +229,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -429,8 +267,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B46549-24DB-F147-A6C4-3602763BDF26}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="206" zoomScaleNormal="206" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" zoomScaleNormal="206" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,239 +598,176 @@
     <col min="4" max="4" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>105</v>
       </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>386</v>
       </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>383</v>
       </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>603</v>
       </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>111</v>
       </c>
-      <c r="D6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>203</v>
       </c>
-      <c r="D7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>404</v>
       </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>103</v>
       </c>
-      <c r="D9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>47</v>
       </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>328</v>
       </c>
-      <c r="D12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>205</v>
       </c>
-      <c r="D13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>109</v>
       </c>
-      <c r="D14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15">
         <v>50</v>
       </c>
-      <c r="D15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>926</v>
       </c>
-      <c r="D17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>351</v>
       </c>
-      <c r="D18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>490</v>
       </c>
-      <c r="D19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>21</v>
       </c>
-      <c r="D20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21">
         <v>652</v>
       </c>
-      <c r="D21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -998,144 +776,105 @@
       <c r="C22" t="s">
         <v>62</v>
       </c>
-      <c r="D22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23">
         <v>67</v>
       </c>
-      <c r="D23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24">
         <v>84</v>
       </c>
-      <c r="D24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25">
         <v>310</v>
       </c>
-      <c r="D25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B26">
         <v>162</v>
       </c>
-      <c r="D26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27">
         <v>78</v>
       </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28">
         <v>243</v>
       </c>
-      <c r="D28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29">
         <v>90</v>
       </c>
-      <c r="D29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30">
         <v>22</v>
       </c>
-      <c r="D30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31">
         <v>81</v>
       </c>
-      <c r="D31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32">
         <v>51</v>
       </c>
-      <c r="D32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33">
         <v>249</v>
       </c>
-      <c r="D33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34">
         <v>118</v>
       </c>
-      <c r="D34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35">
@@ -1144,294 +883,216 @@
       <c r="C35" t="s">
         <v>61</v>
       </c>
-      <c r="D35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36">
         <v>225</v>
       </c>
-      <c r="D36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37">
         <v>99</v>
       </c>
-      <c r="D37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38">
         <v>43</v>
       </c>
-      <c r="D38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39">
         <v>104</v>
       </c>
-      <c r="D39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40">
         <v>97</v>
       </c>
-      <c r="D40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B41">
         <v>184</v>
       </c>
-      <c r="D41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B42">
         <v>63</v>
       </c>
-      <c r="D42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B43">
         <v>259</v>
       </c>
-      <c r="D43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B44">
         <v>284</v>
       </c>
-      <c r="D44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B45">
         <v>499</v>
       </c>
-      <c r="D45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B46">
         <v>308</v>
       </c>
-      <c r="D46" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B47">
         <v>22</v>
       </c>
-      <c r="D47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B48">
         <v>30</v>
       </c>
-      <c r="D48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B49">
         <v>381</v>
       </c>
-      <c r="D49" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B50">
         <v>117</v>
       </c>
-      <c r="D50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B51">
         <v>411</v>
       </c>
-      <c r="D51" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B52">
         <v>461</v>
       </c>
-      <c r="D52" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B53">
         <v>92</v>
       </c>
-      <c r="D53" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B54">
         <v>178</v>
       </c>
-      <c r="D54" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B55">
         <v>368</v>
       </c>
-      <c r="D55" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B56">
         <v>52</v>
       </c>
-      <c r="D56" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B57">
         <v>33</v>
       </c>
-      <c r="D57" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B58">
         <v>32</v>
       </c>
-      <c r="D58" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B59">
         <v>108</v>
       </c>
-      <c r="D59" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B60">
         <v>82</v>
       </c>
-      <c r="D60" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B61">
         <v>254</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63">
         <f>(SUM(B1:B61))</f>
         <v>12016</v>

</xml_diff>